<commit_message>
header, footer, rendered, exportable周り実装
</commit_message>
<xml_diff>
--- a/src/main/resources/DefaultTemplate.xlsx
+++ b/src/main/resources/DefaultTemplate.xlsx
@@ -20,11 +20,11 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>TODO header</t>
+    <t>$C[]{headers}</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>TODO footer</t>
+    <t>$C[]{footers}</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -48,15 +48,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -64,12 +70,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -381,17 +404,17 @@
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>